<commit_message>
Terminamos el historial diario
Se termina el historial diario, es decir la capacidad de guardas, conectarte en el mismo día y tenerlo todo al volver a iniciar sesión
</commit_message>
<xml_diff>
--- a/Historial.xlsx
+++ b/Historial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>2019-05-15</t>
+  </si>
+  <si>
+    <t>2019-05-16</t>
+  </si>
+  <si>
+    <t>leche de soja con copos de maiz</t>
   </si>
   <si>
     <t>leche con avena</t>
@@ -401,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,24 +447,29 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>1234</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>